<commit_message>
#41 fixed NPE in column guesser
</commit_message>
<xml_diff>
--- a/org.polymap.p4/resources-test/simple.xlsx
+++ b/org.polymap.p4/resources-test/simple.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>h2</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>z14</t>
-  </si>
-  <si>
-    <t>z16</t>
   </si>
   <si>
     <t>z17</t>
@@ -187,17 +184,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -527,17 +532,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C18"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -551,10 +556,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -562,10 +567,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -576,7 +581,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -584,10 +589,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
         <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -595,87 +600,87 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
         <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
         <v>33</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>34</v>
-      </c>
-      <c r="C7" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
         <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
         <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
         <v>27</v>
-      </c>
-      <c r="C11" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -683,54 +688,43 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
         <v>17</v>
       </c>
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
         <v>19</v>
       </c>
-      <c r="B16" t="s">
-        <v>20</v>
-      </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
         <v>34</v>
       </c>
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
       <c r="C17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#41 introduce refine guess values
</commit_message>
<xml_diff>
--- a/org.polymap.p4/resources-test/simple.xlsx
+++ b/org.polymap.p4/resources-test/simple.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>h2</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>z14</t>
-  </si>
-  <si>
-    <t>z16</t>
   </si>
   <si>
     <t>z17</t>
@@ -187,17 +184,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -527,17 +532,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C18"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -551,10 +556,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -562,10 +567,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -576,7 +581,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -584,10 +589,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
         <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -595,87 +600,87 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
         <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
         <v>33</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>34</v>
-      </c>
-      <c r="C7" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
         <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
         <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
         <v>27</v>
-      </c>
-      <c r="C11" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -683,54 +688,43 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
         <v>17</v>
       </c>
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
         <v>19</v>
       </c>
-      <c r="B16" t="s">
-        <v>20</v>
-      </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
         <v>34</v>
       </c>
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
       <c r="C17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>